<commit_message>
did a lot of stuff, sorry, my git discipline is not good
</commit_message>
<xml_diff>
--- a/system_rules.xlsx
+++ b/system_rules.xlsx
@@ -178,7 +178,7 @@
     <t xml:space="preserve">R:Theme</t>
   </si>
   <si>
-    <t xml:space="preserve">Capex.*</t>
+    <t xml:space="preserve">r:Capex.*</t>
   </si>
   <si>
     <t xml:space="preserve">Exchange</t>
@@ -202,22 +202,22 @@
     <t xml:space="preserve">If not filled, the Region is the exchange</t>
   </si>
   <si>
-    <t xml:space="preserve">$=TSE|TSX|VENTURE</t>
+    <t xml:space="preserve">r:TSE|TSX|VENTURE</t>
   </si>
   <si>
     <t xml:space="preserve">Canada</t>
   </si>
   <si>
-    <t xml:space="preserve">$=NYSE|NASDAQ|ARCA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$=Eurex</t>
+    <t xml:space="preserve">r:NYSE|NASDAQ|ARCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r:Eurex</t>
   </si>
   <si>
     <t xml:space="preserve">Europe</t>
   </si>
   <si>
-    <t xml:space="preserve">$=SBF|EPA</t>
+    <t xml:space="preserve">r:SBF|EPA</t>
   </si>
   <si>
     <t xml:space="preserve">France</t>
@@ -350,11 +350,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>

</xml_diff>

<commit_message>
now prints picks with no holdings
</commit_message>
<xml_diff>
--- a/system_rules.xlsx
+++ b/system_rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="68">
   <si>
     <t xml:space="preserve">Rules are processed in order</t>
   </si>
@@ -169,13 +169,16 @@
     <t xml:space="preserve">Ticker</t>
   </si>
   <si>
+    <t xml:space="preserve">R:Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divi</t>
+  </si>
+  <si>
     <t xml:space="preserve">Theme</t>
   </si>
   <si>
     <t xml:space="preserve">${theme}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Theme</t>
   </si>
   <si>
     <t xml:space="preserve">r:Capex.*</t>
@@ -348,13 +351,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ56"/>
+  <dimension ref="A1:AMJ62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B57" activeCellId="0" sqref="B57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -666,13 +669,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>50</v>
@@ -683,154 +686,204 @@
         <v>38</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>21</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>21</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E51" s="1"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>62</v>
+      <c r="B52" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>63</v>
+      <c r="B54" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>65</v>
+      <c r="B56" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
works a lot better now. capex and divi report. still needs some cleanup
</commit_message>
<xml_diff>
--- a/system_rules.xlsx
+++ b/system_rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
   <si>
     <t xml:space="preserve">Rules are processed in order</t>
   </si>
@@ -139,46 +139,55 @@
     <t xml:space="preserve">R:PickType</t>
   </si>
   <si>
+    <t xml:space="preserve">${picktype}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:PickDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${picktype}:${ticker}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CapexDiviPortfolio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${sector}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CapexSkeletonPortfolio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${theme}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theme</t>
+  </si>
+  <si>
     <t xml:space="preserve">CapexTotalPortfolio</t>
   </si>
   <si>
     <t xml:space="preserve">R:PickPriority</t>
   </si>
   <si>
-    <t xml:space="preserve">CapexSkeletonPortfolio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CapexDiviPortfolio</t>
-  </si>
-  <si>
     <t xml:space="preserve">CapexBig5</t>
   </si>
   <si>
     <t xml:space="preserve">CapexClosed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${picktype}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:PickDesc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${picktype}:${ticker}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R:Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Divi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${theme}</t>
   </si>
   <si>
     <t xml:space="preserve">r:Capex.*</t>
@@ -351,13 +360,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ62"/>
+  <dimension ref="A1:AMJ64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40:D40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -584,37 +593,44 @@
       <c r="C24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>2</v>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>3</v>
+        <v>47</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,91 +638,86 @@
         <v>38</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>5</v>
+      <c r="D30" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>50</v>
+      <c r="C38" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,99 +725,91 @@
         <v>38</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="0" t="s">
+      <c r="D42" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>55</v>
+      <c r="C44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>21</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C49" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>21</v>
+      <c r="D51" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,16 +817,13 @@
         <v>17</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="E54" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>33</v>
@@ -839,37 +839,40 @@
       <c r="D56" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E57" s="1"/>
+      <c r="E56" s="0" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>63</v>
+      <c r="B58" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>34</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>17</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,13 +880,27 @@
         <v>17</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got rid of pickpriority, and made sector show up in DiviReport for rows that are also in capgains, skel, or big5
</commit_message>
<xml_diff>
--- a/system_rules.xlsx
+++ b/system_rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t xml:space="preserve">Rules are processed in order</t>
   </si>
@@ -181,22 +181,16 @@
     <t xml:space="preserve">CapexTotalPortfolio</t>
   </si>
   <si>
-    <t xml:space="preserve">R:PickPriority</t>
+    <t xml:space="preserve">r:Capex.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${ex}</t>
   </si>
   <si>
     <t xml:space="preserve">CapexBig5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CapexClosed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r:Capex.*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${ex}</t>
   </si>
   <si>
     <t xml:space="preserve">${ex:[A-Z0-9]+}:${ticker}</t>
@@ -360,13 +354,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ64"/>
+  <dimension ref="A1:AMJ54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -677,230 +671,159 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B37" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>3</v>
+      <c r="B41" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>4</v>
+        <v>57</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B44" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>56</v>
+      <c r="C46" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>58</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>58</v>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>59</v>
+        <v>17</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>60</v>
+      <c r="B54" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D62" s="0" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got run_rules_fast to mostly work, but forgot that a rule changes the input that another rule depends on, thereby only one rule can run at a time, then we have to rematch
</commit_message>
<xml_diff>
--- a/system_rules.xlsx
+++ b/system_rules.xlsx
@@ -184,10 +184,10 @@
     <t xml:space="preserve">r:Capex.*</t>
   </si>
   <si>
+    <t xml:space="preserve">${ex}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exchange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${ex}</t>
   </si>
   <si>
     <t xml:space="preserve">CapexBig5</t>
@@ -356,11 +356,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27:D27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="35:35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -656,6 +656,12 @@
       <c r="B33" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="C33" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -664,12 +670,6 @@
       <c r="B34" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -678,19 +678,25 @@
       <c r="B37" s="0" t="s">
         <v>53</v>
       </c>
+      <c r="C37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="C38" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,12 +706,6 @@
       <c r="B39" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -718,7 +718,7 @@
         <v>17</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,7 +754,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
about to chagne the whole thing to make it simpler
</commit_message>
<xml_diff>
--- a/system_rules.xlsx
+++ b/system_rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
   <si>
     <t xml:space="preserve">Rules are processed in order</t>
   </si>
@@ -127,13 +127,22 @@
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Market Value</t>
+    <t xml:space="preserve">Mkt Val (Market Value)</t>
   </si>
   <si>
     <t xml:space="preserve">\$?${value}</t>
   </si>
   <si>
     <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qty (Quantity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${qty}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity</t>
   </si>
   <si>
     <t xml:space="preserve">R:PickType</t>
@@ -236,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -273,6 +282,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -316,7 +330,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,6 +344,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,13 +372,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ54"/>
+  <dimension ref="A1:AMJ56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="35:35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -570,6 +588,12 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="C22" s="0" t="s">
         <v>27</v>
       </c>
@@ -577,176 +601,175 @@
         <v>26</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="C23" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="A24" s="4"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="B26" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>21</v>
+      <c r="C26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>45</v>
+      <c r="C29" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="0" t="s">
+      <c r="C32" s="0" t="s">
         <v>51</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>21</v>
+      <c r="B36" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,16 +777,13 @@
         <v>17</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,7 +791,7 @@
         <v>17</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>33</v>
@@ -779,37 +799,40 @@
       <c r="D48" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="1"/>
+      <c r="E48" s="0" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>64</v>
+      <c r="B50" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>34</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>17</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -817,13 +840,27 @@
         <v>17</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ability to add notes to each stock
</commit_message>
<xml_diff>
--- a/system_rules.xlsx
+++ b/system_rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t xml:space="preserve">Rules are processed in order</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t xml:space="preserve">Match by Region, USA, Canada, etc. and then by Ticker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R:Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">D:Brokerage</t>
@@ -245,7 +251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -282,11 +288,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,7 +331,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,10 +345,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,13 +369,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ56"/>
+  <dimension ref="A1:AMJ57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.41"/>
@@ -464,403 +461,414 @@
       <c r="AMJ10" s="0"/>
     </row>
     <row r="11" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="C11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="AMJ12" s="0"/>
+    </row>
+    <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="AMJ12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>21</v>
-      </c>
+      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="0" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>30</v>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>34</v>
+      <c r="B18" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="B22" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="C23" s="0" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A24" s="1"/>
+      <c r="C24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="D27" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="0" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>48</v>
+      <c r="B28" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>52</v>
+      <c r="B31" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="0" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>52</v>
+      <c r="B34" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>57</v>
+      <c r="D36" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="C40" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>57</v>
+      <c r="C41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="0" t="s">
+      <c r="C45" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="C47" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" s="0" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="0" t="s">
+      <c r="E49" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>68</v>
+      </c>
       <c r="E51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="0" t="s">
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="C53" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C56" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="0" t="s">
+      <c r="C55" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="0" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>